<commit_message>
Added new files to the Sessoin I
</commit_message>
<xml_diff>
--- a/Sessions/I/Activities/001-Instructor-BarCharts/Solved/Pastries.xlsx
+++ b/Sessions/I/Activities/001-Instructor-BarCharts/Solved/Pastries.xlsx
@@ -5,16 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paularias/Documents/EPIC Journey to Professional Careers/DataVisualization-Curriculum/Sessions/I/Activities/001-Instructor-BarCharts/Solved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paularias/Desktop/DataVisualization-Curriculum-main/Sessions/I/Activities/001-Instructor-BarCharts/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45636654-3D44-AB41-B568-2A6D7446C436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066BCE1D-D8D2-6545-ABAA-30784EBF5F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="2420" windowWidth="28040" windowHeight="17440" xr2:uid="{4E5CD058-A6B0-3D46-A85D-7C1EDD44FEB1}"/>
+    <workbookView xWindow="1140" yWindow="-34680" windowWidth="45940" windowHeight="31600" xr2:uid="{4E5CD058-A6B0-3D46-A85D-7C1EDD44FEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$15</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$2:$B$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -135,6 +147,1165 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Favorites</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Favorites</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="42000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="68000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="93000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:tint val="81000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:tint val="69000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:tint val="56000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:tint val="43000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-090D-0D46-975A-C8A5C57D9EC3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Pain aux Raisins</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Caramel Almond Danish</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tiramisu Tart</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Very Berry Pastry</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Savory Mushroom Pastry</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Savory Roasted Vegetable Pastry</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cream Cheese Pastry</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Chocolate Croissant</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Plain Croissant</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sausage Breakfast Pastry</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-54BF-A94E-8B7A-481162DF22E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="19"/>
+        <c:axId val="489639071"/>
+        <c:axId val="489640527"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="489639071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489640527"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="489640527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489639071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1024598</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>754062</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>6613</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E366AC7-F897-8A0D-C35A-AAC04049F946}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,12 +1603,298 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF515BA1-85B7-1C4D-82B8-B7E4257A2E3C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,10 +1916,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -470,10 +1927,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -481,21 +1938,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -536,10 +1993,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -547,10 +2004,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -558,13 +2015,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -579,6 +2036,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C15" xr:uid="{EF515BA1-85B7-1C4D-82B8-B7E4257A2E3C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
+    <sortCondition ref="B1:B14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>